<commit_message>
maj sortie avec 15 observations
</commit_message>
<xml_diff>
--- a/sortie.xlsx
+++ b/sortie.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -297,6 +297,42 @@
   </si>
   <si>
     <t xml:space="preserve">Le verbe "questionner" peut être interprété de plusieurs manières différentes et la terminologie "gestes professionnels" devrait sans doute être précisé ici (pour que toutes et tous comprennent la même chose). Merci.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maud.bouxirot@edufr.ch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">be</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ariane.paccaud@phzh.ch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ju</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nicolas.jobin@unifr.ch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cedjacquier@yahoo.fr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">il s'agirait d'être clair... quelles ressources? quels moyens? quelles compétences? ces termes sont très vastes...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L'idée de "témoigner" de compétences ne m'est pas familière... parlez-vous d'auto-évaluation, de productions écrites ou orales....?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A quelles barrières à l'apprentissages faites-vous allusion? Les obstacles en lien avec les élèves, les enseignants, le programme, la configuration de la classe...?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Même remarque que pour l'item commenté plus haut avec le fait de "témoigner" de ses apprentissages.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Même remarque que celle en lien avec le fait de témoigner ou d'exprimer ses compétences. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">erica.borloz@hepvs.ch</t>
   </si>
 </sst>
 </file>
@@ -2576,6 +2612,1158 @@
         <v>73</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>45</v>
+      </c>
+      <c r="B11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>44301.9213541667</v>
+      </c>
+      <c r="D11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" t="n">
+        <v>1</v>
+      </c>
+      <c r="I11" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" t="n">
+        <v>4</v>
+      </c>
+      <c r="K11" t="n">
+        <v>1</v>
+      </c>
+      <c r="L11" t="n">
+        <v>4</v>
+      </c>
+      <c r="M11" t="n">
+        <v>1</v>
+      </c>
+      <c r="N11" t="n">
+        <v>4</v>
+      </c>
+      <c r="O11" t="n">
+        <v>3</v>
+      </c>
+      <c r="P11" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>2</v>
+      </c>
+      <c r="R11" t="n">
+        <v>4</v>
+      </c>
+      <c r="S11" t="n">
+        <v>1</v>
+      </c>
+      <c r="T11" t="n">
+        <v>4</v>
+      </c>
+      <c r="U11" t="n">
+        <v>1</v>
+      </c>
+      <c r="V11" t="n">
+        <v>4</v>
+      </c>
+      <c r="W11" t="n">
+        <v>1</v>
+      </c>
+      <c r="X11" t="n">
+        <v>4</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>4</v>
+      </c>
+      <c r="AC11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF11" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG11" t="n">
+        <v>2</v>
+      </c>
+      <c r="AH11" t="n">
+        <v>4</v>
+      </c>
+      <c r="AI11" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ11" t="n">
+        <v>4</v>
+      </c>
+      <c r="AK11" t="n">
+        <v>2</v>
+      </c>
+      <c r="AL11" t="n">
+        <v>4</v>
+      </c>
+      <c r="AM11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN11" t="n">
+        <v>4</v>
+      </c>
+      <c r="AO11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP11" t="n">
+        <v>4</v>
+      </c>
+      <c r="AQ11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR11" t="n">
+        <v>4</v>
+      </c>
+      <c r="AS11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT11" t="n">
+        <v>4</v>
+      </c>
+      <c r="AU11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV11" t="n">
+        <v>4</v>
+      </c>
+      <c r="AW11"/>
+      <c r="AX11" t="s">
+        <v>73</v>
+      </c>
+      <c r="AY11" t="s">
+        <v>73</v>
+      </c>
+      <c r="AZ11"/>
+      <c r="BA11" t="s">
+        <v>73</v>
+      </c>
+      <c r="BB11"/>
+      <c r="BC11"/>
+      <c r="BD11"/>
+      <c r="BE11"/>
+      <c r="BF11"/>
+      <c r="BG11" t="s">
+        <v>73</v>
+      </c>
+      <c r="BH11" t="s">
+        <v>73</v>
+      </c>
+      <c r="BI11" t="s">
+        <v>73</v>
+      </c>
+      <c r="BJ11" t="s">
+        <v>73</v>
+      </c>
+      <c r="BK11"/>
+      <c r="BL11"/>
+      <c r="BM11" t="s">
+        <v>73</v>
+      </c>
+      <c r="BN11"/>
+      <c r="BO11" t="s">
+        <v>73</v>
+      </c>
+      <c r="BP11" t="s">
+        <v>73</v>
+      </c>
+      <c r="BQ11" t="s">
+        <v>75</v>
+      </c>
+      <c r="BR11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>47</v>
+      </c>
+      <c r="B12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>44303.3919560185</v>
+      </c>
+      <c r="D12" t="n">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>71</v>
+      </c>
+      <c r="F12" t="s">
+        <v>96</v>
+      </c>
+      <c r="G12" t="n">
+        <v>2</v>
+      </c>
+      <c r="H12" t="n">
+        <v>3</v>
+      </c>
+      <c r="I12" t="n">
+        <v>4</v>
+      </c>
+      <c r="J12" t="n">
+        <v>4</v>
+      </c>
+      <c r="K12" t="n">
+        <v>4</v>
+      </c>
+      <c r="L12" t="n">
+        <v>3</v>
+      </c>
+      <c r="M12" t="n">
+        <v>4</v>
+      </c>
+      <c r="N12" t="n">
+        <v>4</v>
+      </c>
+      <c r="O12" t="n">
+        <v>4</v>
+      </c>
+      <c r="P12" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>3</v>
+      </c>
+      <c r="R12" t="n">
+        <v>4</v>
+      </c>
+      <c r="S12" t="n">
+        <v>4</v>
+      </c>
+      <c r="T12" t="n">
+        <v>4</v>
+      </c>
+      <c r="U12" t="n">
+        <v>3</v>
+      </c>
+      <c r="V12" t="n">
+        <v>4</v>
+      </c>
+      <c r="W12" t="n">
+        <v>4</v>
+      </c>
+      <c r="X12" t="n">
+        <v>4</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB12" t="n">
+        <v>4</v>
+      </c>
+      <c r="AC12" t="n">
+        <v>3</v>
+      </c>
+      <c r="AD12" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE12" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF12" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG12" t="n">
+        <v>3</v>
+      </c>
+      <c r="AH12" t="n">
+        <v>4</v>
+      </c>
+      <c r="AI12" t="n">
+        <v>3</v>
+      </c>
+      <c r="AJ12" t="n">
+        <v>4</v>
+      </c>
+      <c r="AK12" t="n">
+        <v>3</v>
+      </c>
+      <c r="AL12" t="n">
+        <v>4</v>
+      </c>
+      <c r="AM12" t="n">
+        <v>3</v>
+      </c>
+      <c r="AN12" t="n">
+        <v>4</v>
+      </c>
+      <c r="AO12" t="n">
+        <v>4</v>
+      </c>
+      <c r="AP12" t="n">
+        <v>4</v>
+      </c>
+      <c r="AQ12" t="n">
+        <v>4</v>
+      </c>
+      <c r="AR12" t="n">
+        <v>4</v>
+      </c>
+      <c r="AS12" t="n">
+        <v>4</v>
+      </c>
+      <c r="AT12" t="n">
+        <v>4</v>
+      </c>
+      <c r="AU12" t="n">
+        <v>4</v>
+      </c>
+      <c r="AV12" t="n">
+        <v>4</v>
+      </c>
+      <c r="AW12"/>
+      <c r="AX12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AY12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AZ12"/>
+      <c r="BA12" t="s">
+        <v>73</v>
+      </c>
+      <c r="BB12"/>
+      <c r="BC12"/>
+      <c r="BD12"/>
+      <c r="BE12"/>
+      <c r="BF12"/>
+      <c r="BG12" t="s">
+        <v>73</v>
+      </c>
+      <c r="BH12" t="s">
+        <v>73</v>
+      </c>
+      <c r="BI12" t="s">
+        <v>73</v>
+      </c>
+      <c r="BJ12" t="s">
+        <v>73</v>
+      </c>
+      <c r="BK12"/>
+      <c r="BL12"/>
+      <c r="BM12" t="s">
+        <v>73</v>
+      </c>
+      <c r="BN12"/>
+      <c r="BO12" t="s">
+        <v>73</v>
+      </c>
+      <c r="BP12" t="s">
+        <v>73</v>
+      </c>
+      <c r="BQ12" t="s">
+        <v>75</v>
+      </c>
+      <c r="BR12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>48</v>
+      </c>
+      <c r="B13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>44303.4591666667</v>
+      </c>
+      <c r="D13" t="n">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" t="s">
+        <v>98</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" t="n">
+        <v>3</v>
+      </c>
+      <c r="I13" t="n">
+        <v>4</v>
+      </c>
+      <c r="J13" t="n">
+        <v>4</v>
+      </c>
+      <c r="K13" t="n">
+        <v>3</v>
+      </c>
+      <c r="L13" t="n">
+        <v>3</v>
+      </c>
+      <c r="M13" t="n">
+        <v>4</v>
+      </c>
+      <c r="N13" t="n">
+        <v>4</v>
+      </c>
+      <c r="O13" t="n">
+        <v>4</v>
+      </c>
+      <c r="P13" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>4</v>
+      </c>
+      <c r="R13" t="n">
+        <v>4</v>
+      </c>
+      <c r="S13" t="n">
+        <v>4</v>
+      </c>
+      <c r="T13" t="n">
+        <v>3</v>
+      </c>
+      <c r="U13" t="n">
+        <v>3</v>
+      </c>
+      <c r="V13" t="n">
+        <v>3</v>
+      </c>
+      <c r="W13" t="n">
+        <v>3</v>
+      </c>
+      <c r="X13" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>3</v>
+      </c>
+      <c r="AD13" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE13" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF13" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG13" t="n">
+        <v>3</v>
+      </c>
+      <c r="AH13" t="n">
+        <v>3</v>
+      </c>
+      <c r="AI13" t="n">
+        <v>3</v>
+      </c>
+      <c r="AJ13" t="n">
+        <v>4</v>
+      </c>
+      <c r="AK13" t="n">
+        <v>3</v>
+      </c>
+      <c r="AL13" t="n">
+        <v>3</v>
+      </c>
+      <c r="AM13" t="n">
+        <v>4</v>
+      </c>
+      <c r="AN13" t="n">
+        <v>4</v>
+      </c>
+      <c r="AO13" t="n">
+        <v>3</v>
+      </c>
+      <c r="AP13" t="n">
+        <v>3</v>
+      </c>
+      <c r="AQ13" t="n">
+        <v>4</v>
+      </c>
+      <c r="AR13" t="n">
+        <v>4</v>
+      </c>
+      <c r="AS13" t="n">
+        <v>3</v>
+      </c>
+      <c r="AT13" t="n">
+        <v>3</v>
+      </c>
+      <c r="AU13" t="n">
+        <v>3</v>
+      </c>
+      <c r="AV13" t="n">
+        <v>4</v>
+      </c>
+      <c r="AW13"/>
+      <c r="AX13" t="s">
+        <v>73</v>
+      </c>
+      <c r="AY13" t="s">
+        <v>73</v>
+      </c>
+      <c r="AZ13"/>
+      <c r="BA13" t="s">
+        <v>73</v>
+      </c>
+      <c r="BB13"/>
+      <c r="BC13"/>
+      <c r="BD13"/>
+      <c r="BE13"/>
+      <c r="BF13"/>
+      <c r="BG13" t="s">
+        <v>73</v>
+      </c>
+      <c r="BH13" t="s">
+        <v>73</v>
+      </c>
+      <c r="BI13" t="s">
+        <v>73</v>
+      </c>
+      <c r="BJ13" t="s">
+        <v>73</v>
+      </c>
+      <c r="BK13"/>
+      <c r="BL13"/>
+      <c r="BM13" t="s">
+        <v>73</v>
+      </c>
+      <c r="BN13"/>
+      <c r="BO13" t="s">
+        <v>73</v>
+      </c>
+      <c r="BP13" t="s">
+        <v>73</v>
+      </c>
+      <c r="BQ13" t="s">
+        <v>75</v>
+      </c>
+      <c r="BR13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>49</v>
+      </c>
+      <c r="B14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>44305.7788773148</v>
+      </c>
+      <c r="D14" t="n">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F14" t="s">
+        <v>72</v>
+      </c>
+      <c r="G14" t="n">
+        <v>3</v>
+      </c>
+      <c r="H14" t="n">
+        <v>2</v>
+      </c>
+      <c r="I14" t="n">
+        <v>4</v>
+      </c>
+      <c r="J14" t="n">
+        <v>4</v>
+      </c>
+      <c r="K14" t="n">
+        <v>4</v>
+      </c>
+      <c r="L14" t="n">
+        <v>4</v>
+      </c>
+      <c r="M14" t="n">
+        <v>4</v>
+      </c>
+      <c r="N14" t="n">
+        <v>4</v>
+      </c>
+      <c r="O14" t="n">
+        <v>2</v>
+      </c>
+      <c r="P14" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>4</v>
+      </c>
+      <c r="R14" t="n">
+        <v>4</v>
+      </c>
+      <c r="S14" t="n">
+        <v>4</v>
+      </c>
+      <c r="T14" t="n">
+        <v>4</v>
+      </c>
+      <c r="U14" t="n">
+        <v>4</v>
+      </c>
+      <c r="V14" t="n">
+        <v>4</v>
+      </c>
+      <c r="W14" t="n">
+        <v>4</v>
+      </c>
+      <c r="X14" t="n">
+        <v>4</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA14" t="n">
+        <v>4</v>
+      </c>
+      <c r="AB14" t="n">
+        <v>4</v>
+      </c>
+      <c r="AC14" t="n">
+        <v>3</v>
+      </c>
+      <c r="AD14" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE14" t="n">
+        <v>4</v>
+      </c>
+      <c r="AF14" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG14" t="n">
+        <v>4</v>
+      </c>
+      <c r="AH14" t="n">
+        <v>4</v>
+      </c>
+      <c r="AI14" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ14" t="n">
+        <v>4</v>
+      </c>
+      <c r="AK14" t="n">
+        <v>4</v>
+      </c>
+      <c r="AL14" t="n">
+        <v>4</v>
+      </c>
+      <c r="AM14" t="n">
+        <v>4</v>
+      </c>
+      <c r="AN14" t="n">
+        <v>4</v>
+      </c>
+      <c r="AO14" t="n">
+        <v>4</v>
+      </c>
+      <c r="AP14" t="n">
+        <v>4</v>
+      </c>
+      <c r="AQ14" t="n">
+        <v>4</v>
+      </c>
+      <c r="AR14" t="n">
+        <v>4</v>
+      </c>
+      <c r="AS14" t="n">
+        <v>4</v>
+      </c>
+      <c r="AT14" t="n">
+        <v>4</v>
+      </c>
+      <c r="AU14" t="n">
+        <v>4</v>
+      </c>
+      <c r="AV14" t="n">
+        <v>4</v>
+      </c>
+      <c r="AW14"/>
+      <c r="AX14" t="s">
+        <v>73</v>
+      </c>
+      <c r="AY14" t="s">
+        <v>73</v>
+      </c>
+      <c r="AZ14"/>
+      <c r="BA14" t="s">
+        <v>73</v>
+      </c>
+      <c r="BB14"/>
+      <c r="BC14"/>
+      <c r="BD14"/>
+      <c r="BE14"/>
+      <c r="BF14"/>
+      <c r="BG14" t="s">
+        <v>73</v>
+      </c>
+      <c r="BH14" t="s">
+        <v>73</v>
+      </c>
+      <c r="BI14" t="s">
+        <v>73</v>
+      </c>
+      <c r="BJ14" t="s">
+        <v>73</v>
+      </c>
+      <c r="BK14"/>
+      <c r="BL14"/>
+      <c r="BM14" t="s">
+        <v>73</v>
+      </c>
+      <c r="BN14"/>
+      <c r="BO14" t="s">
+        <v>73</v>
+      </c>
+      <c r="BP14" t="s">
+        <v>73</v>
+      </c>
+      <c r="BQ14" t="s">
+        <v>75</v>
+      </c>
+      <c r="BR14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>51</v>
+      </c>
+      <c r="B15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>44309.3693518519</v>
+      </c>
+      <c r="D15" t="n">
+        <v>3</v>
+      </c>
+      <c r="E15" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" t="s">
+        <v>72</v>
+      </c>
+      <c r="G15" t="n">
+        <v>3</v>
+      </c>
+      <c r="H15" t="n">
+        <v>2</v>
+      </c>
+      <c r="I15" t="n">
+        <v>4</v>
+      </c>
+      <c r="J15" t="n">
+        <v>4</v>
+      </c>
+      <c r="K15" t="n">
+        <v>4</v>
+      </c>
+      <c r="L15" t="n">
+        <v>4</v>
+      </c>
+      <c r="M15" t="n">
+        <v>4</v>
+      </c>
+      <c r="N15" t="n">
+        <v>4</v>
+      </c>
+      <c r="O15" t="n">
+        <v>4</v>
+      </c>
+      <c r="P15" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>3</v>
+      </c>
+      <c r="R15" t="n">
+        <v>3</v>
+      </c>
+      <c r="S15" t="n">
+        <v>4</v>
+      </c>
+      <c r="T15" t="n">
+        <v>3</v>
+      </c>
+      <c r="U15" t="n">
+        <v>4</v>
+      </c>
+      <c r="V15" t="n">
+        <v>4</v>
+      </c>
+      <c r="W15" t="n">
+        <v>4</v>
+      </c>
+      <c r="X15" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z15" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA15" t="n">
+        <v>4</v>
+      </c>
+      <c r="AB15" t="n">
+        <v>4</v>
+      </c>
+      <c r="AC15" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD15" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE15" t="n">
+        <v>4</v>
+      </c>
+      <c r="AF15" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG15" t="n">
+        <v>4</v>
+      </c>
+      <c r="AH15" t="n">
+        <v>3</v>
+      </c>
+      <c r="AI15" t="n">
+        <v>3</v>
+      </c>
+      <c r="AJ15" t="n">
+        <v>2</v>
+      </c>
+      <c r="AK15" t="n">
+        <v>4</v>
+      </c>
+      <c r="AL15" t="n">
+        <v>3</v>
+      </c>
+      <c r="AM15" t="n">
+        <v>4</v>
+      </c>
+      <c r="AN15" t="n">
+        <v>4</v>
+      </c>
+      <c r="AO15" t="n">
+        <v>3</v>
+      </c>
+      <c r="AP15" t="n">
+        <v>3</v>
+      </c>
+      <c r="AQ15" t="n">
+        <v>4</v>
+      </c>
+      <c r="AR15" t="n">
+        <v>4</v>
+      </c>
+      <c r="AS15" t="n">
+        <v>4</v>
+      </c>
+      <c r="AT15" t="n">
+        <v>4</v>
+      </c>
+      <c r="AU15" t="n">
+        <v>4</v>
+      </c>
+      <c r="AV15" t="n">
+        <v>3</v>
+      </c>
+      <c r="AW15"/>
+      <c r="AX15" t="s">
+        <v>73</v>
+      </c>
+      <c r="AY15" t="s">
+        <v>73</v>
+      </c>
+      <c r="AZ15"/>
+      <c r="BA15" t="s">
+        <v>73</v>
+      </c>
+      <c r="BB15"/>
+      <c r="BC15"/>
+      <c r="BD15"/>
+      <c r="BE15"/>
+      <c r="BF15"/>
+      <c r="BG15" t="s">
+        <v>101</v>
+      </c>
+      <c r="BH15" t="s">
+        <v>73</v>
+      </c>
+      <c r="BI15" t="s">
+        <v>73</v>
+      </c>
+      <c r="BJ15" t="s">
+        <v>101</v>
+      </c>
+      <c r="BK15"/>
+      <c r="BL15"/>
+      <c r="BM15" t="s">
+        <v>73</v>
+      </c>
+      <c r="BN15"/>
+      <c r="BO15" t="s">
+        <v>73</v>
+      </c>
+      <c r="BP15" t="s">
+        <v>73</v>
+      </c>
+      <c r="BQ15" t="s">
+        <v>80</v>
+      </c>
+      <c r="BR15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>52</v>
+      </c>
+      <c r="B16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>44309.8508333333</v>
+      </c>
+      <c r="D16" t="n">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" t="s">
+        <v>72</v>
+      </c>
+      <c r="G16" t="n">
+        <v>3</v>
+      </c>
+      <c r="H16" t="n">
+        <v>3</v>
+      </c>
+      <c r="I16" t="n">
+        <v>4</v>
+      </c>
+      <c r="J16" t="n">
+        <v>4</v>
+      </c>
+      <c r="K16" t="n">
+        <v>4</v>
+      </c>
+      <c r="L16" t="n">
+        <v>4</v>
+      </c>
+      <c r="M16" t="n">
+        <v>4</v>
+      </c>
+      <c r="N16" t="n">
+        <v>4</v>
+      </c>
+      <c r="O16" t="n">
+        <v>2</v>
+      </c>
+      <c r="P16" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>3</v>
+      </c>
+      <c r="R16" t="n">
+        <v>4</v>
+      </c>
+      <c r="S16" t="n">
+        <v>4</v>
+      </c>
+      <c r="T16" t="n">
+        <v>4</v>
+      </c>
+      <c r="U16" t="n">
+        <v>4</v>
+      </c>
+      <c r="V16" t="n">
+        <v>4</v>
+      </c>
+      <c r="W16" t="n">
+        <v>3</v>
+      </c>
+      <c r="X16" t="n">
+        <v>4</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA16" t="n">
+        <v>4</v>
+      </c>
+      <c r="AB16" t="n">
+        <v>4</v>
+      </c>
+      <c r="AC16" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE16" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF16" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG16" t="n">
+        <v>3</v>
+      </c>
+      <c r="AH16" t="n">
+        <v>2</v>
+      </c>
+      <c r="AI16" t="n">
+        <v>3</v>
+      </c>
+      <c r="AJ16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK16" t="n">
+        <v>4</v>
+      </c>
+      <c r="AL16" t="n">
+        <v>4</v>
+      </c>
+      <c r="AM16" t="n">
+        <v>4</v>
+      </c>
+      <c r="AN16" t="n">
+        <v>4</v>
+      </c>
+      <c r="AO16" t="n">
+        <v>4</v>
+      </c>
+      <c r="AP16" t="n">
+        <v>4</v>
+      </c>
+      <c r="AQ16" t="n">
+        <v>4</v>
+      </c>
+      <c r="AR16" t="n">
+        <v>4</v>
+      </c>
+      <c r="AS16" t="n">
+        <v>4</v>
+      </c>
+      <c r="AT16" t="n">
+        <v>3</v>
+      </c>
+      <c r="AU16" t="n">
+        <v>4</v>
+      </c>
+      <c r="AV16" t="n">
+        <v>4</v>
+      </c>
+      <c r="AW16"/>
+      <c r="AX16" t="s">
+        <v>73</v>
+      </c>
+      <c r="AY16" t="s">
+        <v>73</v>
+      </c>
+      <c r="AZ16"/>
+      <c r="BA16" t="s">
+        <v>73</v>
+      </c>
+      <c r="BB16"/>
+      <c r="BC16"/>
+      <c r="BD16"/>
+      <c r="BE16"/>
+      <c r="BF16"/>
+      <c r="BG16" t="s">
+        <v>102</v>
+      </c>
+      <c r="BH16" t="s">
+        <v>103</v>
+      </c>
+      <c r="BI16" t="s">
+        <v>104</v>
+      </c>
+      <c r="BJ16" t="s">
+        <v>105</v>
+      </c>
+      <c r="BK16"/>
+      <c r="BL16"/>
+      <c r="BM16" t="s">
+        <v>73</v>
+      </c>
+      <c r="BN16"/>
+      <c r="BO16" t="s">
+        <v>73</v>
+      </c>
+      <c r="BP16" t="s">
+        <v>73</v>
+      </c>
+      <c r="BQ16" t="s">
+        <v>75</v>
+      </c>
+      <c r="BR16" t="s">
+        <v>106</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>